<commit_message>
All projects working (except dynamic pricing, project 7)
</commit_message>
<xml_diff>
--- a/docs/spreadsheet illustrations.xlsx
+++ b/docs/spreadsheet illustrations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25602" windowHeight="10380" firstSheet="1" activeTab="1" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25602" windowHeight="10380" activeTab="2" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Reproduction" sheetId="9" r:id="rId1"/>
@@ -1422,9 +1422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982C02D3-D3A2-4B19-B233-AA79ED6FA192}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:P25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1697,9 +1695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECE59FE-C8CF-46B2-8E67-2ECAE9AA0094}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1977,8 +1973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFFBB03-2118-4987-A5B0-62F260E68AFF}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Save and validate working, very minor bug
</commit_message>
<xml_diff>
--- a/docs/spreadsheet illustrations.xlsx
+++ b/docs/spreadsheet illustrations.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afree\eclipse-workspace\capitalism-9.0\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA01C68-E24D-4130-A713-F324D2975AB6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25602" windowHeight="10380" firstSheet="1" activeTab="7" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25602" windowHeight="10380" firstSheet="1" activeTab="3" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Reproduction" sheetId="9" r:id="rId1"/>
@@ -741,9 +742,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
@@ -796,39 +794,42 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2494,10 +2495,10 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="18"/>
+      <c r="H4" s="60"/>
     </row>
     <row r="5" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="6" t="s">
@@ -2733,10 +2734,10 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="18"/>
+      <c r="H12" s="60"/>
     </row>
     <row r="13" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="6" t="s">
@@ -2979,12 +2980,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C77ED3-DCBF-4325-9E6B-9BF828DE079E}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="2" max="2" width="16.15625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.3125" customWidth="1"/>
     <col min="9" max="9" width="13.15625" customWidth="1"/>
   </cols>
@@ -3150,7 +3152,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:E6"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3172,10 +3174,10 @@
         <v>0.1</v>
       </c>
       <c r="N1"/>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="18"/>
+      <c r="Q1" s="60"/>
     </row>
     <row r="2" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" s="6" t="s">
@@ -6087,7 +6089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E95B74-9862-418D-BA3B-462B9CE1D294}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -6103,24 +6105,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="40" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6128,172 +6130,172 @@
       <c r="A3" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="66" t="s">
+      <c r="H3" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="47">
         <v>225</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="29">
         <v>90</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="29">
         <v>60</v>
       </c>
-      <c r="E4" s="65">
+      <c r="E4" s="58">
         <f>B4+C4+D4</f>
         <v>375</v>
       </c>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="47">
         <v>100</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="29">
         <v>120</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="29">
         <v>80</v>
       </c>
-      <c r="E5" s="63">
+      <c r="E5" s="57">
         <f>B5+C5+D5</f>
         <v>300</v>
       </c>
-      <c r="H5" s="62" t="s">
+      <c r="H5" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="48">
+      <c r="B6" s="47">
         <v>50</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="29">
         <v>90</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="29">
         <v>60</v>
       </c>
-      <c r="E6" s="61">
+      <c r="E6" s="56">
         <f>B6+C6+D6</f>
         <v>200</v>
       </c>
-      <c r="H6" s="60" t="s">
+      <c r="H6" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B7" s="55">
         <f>SUM(B4:B6)</f>
         <v>375</v>
       </c>
-      <c r="C7" s="58">
+      <c r="C7" s="54">
         <f>SUM(C4:C6)</f>
         <v>300</v>
       </c>
-      <c r="D7" s="57">
+      <c r="D7" s="53">
         <f>SUM(D4:D6)</f>
         <v>200</v>
       </c>
-      <c r="E7" s="56">
+      <c r="E7" s="52">
         <f>B7+C7+D7</f>
         <v>875</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="53"/>
-      <c r="H9" s="55" t="s">
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="64"/>
+      <c r="H9" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="53"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="64"/>
     </row>
     <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="32" t="s">
         <v>4</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="52" t="s">
+      <c r="H10" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="51" t="s">
+      <c r="I10" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="51" t="s">
+      <c r="J10" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="K10" s="51" t="s">
+      <c r="K10" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="L10" s="51" t="s">
+      <c r="L10" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="M10" s="33" t="s">
+      <c r="M10" s="32" t="s">
         <v>68</v>
       </c>
     </row>
@@ -6301,46 +6303,46 @@
       <c r="A11" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="48">
+      <c r="B11" s="47">
         <v>225</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="29">
         <f>C4+D4</f>
         <v>150</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="31">
         <f>B11+C11</f>
         <v>375</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="29">
         <f>C4</f>
         <v>90</v>
       </c>
-      <c r="F11" s="49">
+      <c r="F11" s="48">
         <f>C11-E11</f>
         <v>60</v>
       </c>
-      <c r="H11" s="48">
+      <c r="H11" s="47">
         <f>B11+E11</f>
         <v>315</v>
       </c>
-      <c r="I11" s="26">
+      <c r="I11" s="25">
         <f>F11/H11</f>
         <v>0.19047619047619047</v>
       </c>
-      <c r="J11" s="26">
+      <c r="J11" s="25">
         <f>H11*I14</f>
         <v>93.333333333333329</v>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="25">
         <f>J11-F11</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="L11" s="28">
+      <c r="L11" s="27">
         <f>B11+E11+J11</f>
         <v>408.33333333333331</v>
       </c>
-      <c r="M11" s="50">
+      <c r="M11" s="49">
         <f>L11/D11</f>
         <v>1.0888888888888888</v>
       </c>
@@ -6352,46 +6354,46 @@
       <c r="A12" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="48">
+      <c r="B12" s="47">
         <v>100</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="29">
         <f>C5+D5</f>
         <v>200</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="30">
         <f>B12+C12</f>
         <v>300</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="29">
         <f>C5</f>
         <v>120</v>
       </c>
-      <c r="F12" s="49">
+      <c r="F12" s="48">
         <f>C12-E12</f>
         <v>80</v>
       </c>
-      <c r="H12" s="48">
+      <c r="H12" s="47">
         <f>B12+E12</f>
         <v>220</v>
       </c>
-      <c r="I12" s="26">
+      <c r="I12" s="25">
         <f>F12/H12</f>
         <v>0.36363636363636365</v>
       </c>
-      <c r="J12" s="26">
+      <c r="J12" s="25">
         <f>H12*I14</f>
         <v>65.185185185185176</v>
       </c>
-      <c r="K12" s="26">
+      <c r="K12" s="25">
         <f>J12-F12</f>
         <v>-14.814814814814824</v>
       </c>
-      <c r="L12" s="28">
+      <c r="L12" s="27">
         <f>B12+E12+J12</f>
         <v>285.18518518518516</v>
       </c>
-      <c r="M12" s="50">
+      <c r="M12" s="49">
         <f>L12/D12</f>
         <v>0.95061728395061718</v>
       </c>
@@ -6403,136 +6405,136 @@
       <c r="A13" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="48">
+      <c r="B13" s="47">
         <v>50</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="29">
         <f>C6+D6</f>
         <v>150</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="28">
         <f>B13+C13</f>
         <v>200</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="29">
         <f>C6</f>
         <v>90</v>
       </c>
-      <c r="F13" s="49">
+      <c r="F13" s="48">
         <f>C13-E13</f>
         <v>60</v>
       </c>
-      <c r="H13" s="48">
+      <c r="H13" s="47">
         <f>B13+E13</f>
         <v>140</v>
       </c>
-      <c r="I13" s="26">
+      <c r="I13" s="25">
         <f>F13/H13</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="J13" s="26">
+      <c r="J13" s="25">
         <f>H13*I14</f>
         <v>41.481481481481481</v>
       </c>
-      <c r="K13" s="26">
+      <c r="K13" s="25">
         <f>J13-F13</f>
         <v>-18.518518518518519</v>
       </c>
-      <c r="L13" s="28">
+      <c r="L13" s="27">
         <f>B13+E13+J13</f>
         <v>181.48148148148147</v>
       </c>
-      <c r="M13" s="47">
+      <c r="M13" s="46">
         <f>L13/D13</f>
         <v>0.90740740740740733</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="23">
         <f>SUM(B11:B13)</f>
         <v>375</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="43">
         <f>SUM(C11:C13)</f>
         <v>500</v>
       </c>
-      <c r="D14" s="44">
+      <c r="D14" s="43">
         <f>SUM(D11:D13)</f>
         <v>875</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="22">
         <f>SUM(E11:E13)</f>
         <v>300</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
         <f>SUM(F11:F13)</f>
         <v>200</v>
       </c>
-      <c r="H14" s="45">
+      <c r="H14" s="44">
         <f>SUM(H11:H13)</f>
         <v>675</v>
       </c>
-      <c r="I14" s="20">
+      <c r="I14" s="19">
         <f>F14/H14</f>
         <v>0.29629629629629628</v>
       </c>
-      <c r="J14" s="44">
+      <c r="J14" s="43">
         <f>SUM(J11:J13)</f>
         <v>200</v>
       </c>
-      <c r="K14" s="44">
+      <c r="K14" s="43">
         <f>SUM(K11:K13)</f>
         <v>0</v>
       </c>
-      <c r="L14" s="44">
+      <c r="L14" s="43">
         <f>SUM(L11:L13)</f>
         <v>875</v>
       </c>
-      <c r="M14" s="43"/>
+      <c r="M14" s="42"/>
     </row>
     <row r="15" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="M15" s="42"/>
+      <c r="M15" s="41"/>
     </row>
     <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="38" t="str">
+      <c r="C16" s="37" t="str">
         <f>C10</f>
         <v>L(=V+S)</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="F16" s="36" t="s">
         <v>4</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="34" t="s">
+      <c r="J16" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="K16" s="34" t="s">
+      <c r="K16" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="L16" s="34" t="s">
+      <c r="L16" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="M16" s="33" t="s">
+      <c r="M16" s="32" t="s">
         <v>68</v>
       </c>
     </row>
@@ -6540,48 +6542,48 @@
       <c r="A17" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="26">
         <f>B11*M11</f>
         <v>244.99999999999997</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="29">
         <f>C11</f>
         <v>150</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="31">
         <f>B17+C17</f>
         <v>395</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="27">
         <f>E11*M12</f>
         <v>85.555555555555543</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="24">
         <f>C17-E17</f>
         <v>64.444444444444457</v>
       </c>
       <c r="G17" s="10"/>
-      <c r="H17" s="27">
+      <c r="H17" s="26">
         <f>B17+E17</f>
         <v>330.55555555555554</v>
       </c>
-      <c r="I17" s="26">
+      <c r="I17" s="25">
         <f>F17/H17</f>
         <v>0.19495798319327737</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="25">
         <f>H17*I20</f>
         <v>102.38836967808932</v>
       </c>
-      <c r="K17" s="26">
+      <c r="K17" s="25">
         <f>J17-F17</f>
         <v>37.943925233644862</v>
       </c>
-      <c r="L17" s="26">
+      <c r="L17" s="25">
         <f>B17+E17+J17</f>
         <v>432.94392523364485</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="24">
         <f>L17/D17</f>
         <v>1.0960605702117592</v>
       </c>
@@ -6590,48 +6592,48 @@
       <c r="A18" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="27">
+      <c r="B18" s="26">
         <f>B12*M11</f>
         <v>108.88888888888889</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="29">
         <f>C12</f>
         <v>200</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="30">
         <f>B18+C18</f>
         <v>308.88888888888891</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="27">
         <f>E12*M12</f>
         <v>114.07407407407406</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="24">
         <f>C18-E18</f>
         <v>85.925925925925938</v>
       </c>
       <c r="G18" s="10"/>
-      <c r="H18" s="27">
+      <c r="H18" s="26">
         <f>B18+E18</f>
         <v>222.96296296296293</v>
       </c>
-      <c r="I18" s="26">
+      <c r="I18" s="25">
         <f>F18/H18</f>
         <v>0.38538205980066453</v>
       </c>
-      <c r="J18" s="26">
+      <c r="J18" s="25">
         <f>H18*I20</f>
         <v>69.0619591554171</v>
       </c>
-      <c r="K18" s="26">
+      <c r="K18" s="25">
         <f>J18-F18</f>
         <v>-16.863966770508839</v>
       </c>
-      <c r="L18" s="26">
+      <c r="L18" s="25">
         <f>B18+E18+J18</f>
         <v>292.02492211838</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="24">
         <f>L18/D18</f>
         <v>0.94540442412425174</v>
       </c>
@@ -6640,95 +6642,95 @@
       <c r="A19" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="26">
         <f>B13*M11</f>
         <v>54.444444444444443</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="29">
         <f>C13</f>
         <v>150</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="28">
         <f>B19+C19</f>
         <v>204.44444444444446</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="27">
         <f>E13*M12</f>
         <v>85.555555555555543</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="24">
         <f>C19-E19</f>
         <v>64.444444444444457</v>
       </c>
       <c r="G19" s="10"/>
-      <c r="H19" s="27">
+      <c r="H19" s="26">
         <f>B19+E19</f>
         <v>140</v>
       </c>
-      <c r="I19" s="26">
+      <c r="I19" s="25">
         <f>F19/H19</f>
         <v>0.4603174603174604</v>
       </c>
-      <c r="J19" s="26">
+      <c r="J19" s="25">
         <f>H19*I20</f>
         <v>43.36448598130842</v>
       </c>
-      <c r="K19" s="26">
+      <c r="K19" s="25">
         <f>J19-F19</f>
         <v>-21.079958463136037</v>
       </c>
-      <c r="L19" s="26">
+      <c r="L19" s="25">
         <f>B19+E19+J19</f>
         <v>183.36448598130841</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="24">
         <f>L19/D19</f>
         <v>0.89689150751726932</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B20" s="24">
+      <c r="B20" s="23">
         <f>SUM(B17:B19)</f>
         <v>408.33333333333331</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="19">
         <f>SUM(C17:C19)</f>
         <v>500</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="19">
         <f>SUM(D17:D19)</f>
         <v>908.33333333333337</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="22">
         <f>SUM(E17:E19)</f>
         <v>285.18518518518516</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="21">
         <f>SUM(F17:F19)</f>
         <v>214.81481481481484</v>
       </c>
       <c r="G20" s="10"/>
-      <c r="H20" s="21">
+      <c r="H20" s="20">
         <f>SUM(H17:H19)</f>
         <v>693.51851851851848</v>
       </c>
-      <c r="I20" s="20">
+      <c r="I20" s="19">
         <f>F20/H20</f>
         <v>0.30974632843791727</v>
       </c>
-      <c r="J20" s="20">
+      <c r="J20" s="19">
         <f>SUM(J17:J19)</f>
         <v>214.81481481481484</v>
       </c>
-      <c r="K20" s="20">
+      <c r="K20" s="19">
         <f>SUM(K17:K19)</f>
         <v>0</v>
       </c>
-      <c r="L20" s="20">
+      <c r="L20" s="19">
         <f>SUM(L17:L19)</f>
         <v>908.33333333333326</v>
       </c>
-      <c r="M20" s="19"/>
+      <c r="M20" s="18"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="H22" s="7" t="s">
@@ -6751,45 +6753,45 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="M26" s="40"/>
+      <c r="M26" s="39"/>
     </row>
     <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="38" t="str">
+      <c r="C27" s="37" t="str">
         <f>C16</f>
         <v>L(=V+S)</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="37" t="s">
+      <c r="F27" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="36"/>
-      <c r="H27" s="35" t="s">
+      <c r="G27" s="35"/>
+      <c r="H27" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="J27" s="34" t="s">
+      <c r="J27" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="K27" s="34" t="s">
+      <c r="K27" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="L27" s="34" t="s">
+      <c r="L27" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="M27" s="33" t="s">
+      <c r="M27" s="32" t="s">
         <v>68</v>
       </c>
     </row>
@@ -6797,48 +6799,48 @@
       <c r="A28" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="26">
         <f>B17*M17</f>
         <v>268.53483970188097</v>
       </c>
-      <c r="C28" s="30">
+      <c r="C28" s="29">
         <f>C17</f>
         <v>150</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="31">
         <f>B28+C28</f>
         <v>418.53483970188097</v>
       </c>
-      <c r="E28" s="28">
+      <c r="E28" s="27">
         <f>E17*$M$12</f>
         <v>81.33058984910835</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="24">
         <f>C28-E28</f>
         <v>68.66941015089165</v>
       </c>
       <c r="G28" s="10"/>
-      <c r="H28" s="27">
+      <c r="H28" s="26">
         <f>B28+E28</f>
         <v>349.86542955098935</v>
       </c>
-      <c r="I28" s="26">
+      <c r="I28" s="25">
         <f>F28/H28</f>
         <v>0.1962737794329113</v>
       </c>
-      <c r="J28" s="26">
+      <c r="J28" s="25">
         <f>H28*I31</f>
         <v>111.43448268784891</v>
       </c>
-      <c r="K28" s="26">
+      <c r="K28" s="25">
         <f>J28-F28</f>
         <v>42.765072536957263</v>
       </c>
-      <c r="L28" s="26">
+      <c r="L28" s="25">
         <f>B28+E28+J28</f>
         <v>461.29991223883826</v>
       </c>
-      <c r="M28" s="25">
+      <c r="M28" s="24">
         <f>L28/D28</f>
         <v>1.1021780470352684</v>
       </c>
@@ -6847,48 +6849,48 @@
       <c r="A29" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="27">
+      <c r="B29" s="26">
         <f>B18*M17</f>
         <v>119.34881764528043</v>
       </c>
-      <c r="C29" s="30">
+      <c r="C29" s="29">
         <f>C18</f>
         <v>200</v>
       </c>
-      <c r="D29" s="31">
+      <c r="D29" s="30">
         <f>B29+C29</f>
         <v>319.34881764528041</v>
       </c>
-      <c r="E29" s="28">
+      <c r="E29" s="27">
         <f>E18*$M$12</f>
         <v>108.4407864654778</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29" s="24">
         <f>C29-E29</f>
         <v>91.5592135345222</v>
       </c>
       <c r="G29" s="10"/>
-      <c r="H29" s="27">
+      <c r="H29" s="26">
         <f>B29+E29</f>
         <v>227.78960411075823</v>
       </c>
-      <c r="I29" s="26">
+      <c r="I29" s="25">
         <f>F29/H29</f>
         <v>0.40194640967900941</v>
       </c>
-      <c r="J29" s="26">
+      <c r="J29" s="25">
         <f>H29*I31</f>
         <v>72.552514629207863</v>
       </c>
-      <c r="K29" s="26">
+      <c r="K29" s="25">
         <f>J29-F29</f>
         <v>-19.006698905314337</v>
       </c>
-      <c r="L29" s="26">
+      <c r="L29" s="25">
         <f>B29+E29+J29</f>
         <v>300.34211873996611</v>
       </c>
-      <c r="M29" s="25">
+      <c r="M29" s="24">
         <f>L29/D29</f>
         <v>0.9404829520100928</v>
       </c>
@@ -6897,95 +6899,95 @@
       <c r="A30" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="27">
+      <c r="B30" s="26">
         <f>B19*M17</f>
         <v>59.674408822640217</v>
       </c>
-      <c r="C30" s="30">
+      <c r="C30" s="29">
         <f>C19</f>
         <v>150</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30" s="28">
         <f>B30+C30</f>
         <v>209.6744088226402</v>
       </c>
-      <c r="E30" s="28">
+      <c r="E30" s="27">
         <f>E19*$M$12</f>
         <v>81.33058984910835</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="24">
         <f>C30-E30</f>
         <v>68.66941015089165</v>
       </c>
       <c r="G30" s="10"/>
-      <c r="H30" s="27">
+      <c r="H30" s="26">
         <f>B30+E30</f>
         <v>141.00499867174858</v>
       </c>
-      <c r="I30" s="26">
+      <c r="I30" s="25">
         <f>F30/H30</f>
         <v>0.48699982835892247</v>
       </c>
-      <c r="J30" s="26">
+      <c r="J30" s="25">
         <f>H30*I31</f>
         <v>44.911036519248732</v>
       </c>
-      <c r="K30" s="26">
+      <c r="K30" s="25">
         <f>J30-F30</f>
         <v>-23.758373631642918</v>
       </c>
-      <c r="L30" s="26">
+      <c r="L30" s="25">
         <f>B30+E30+J30</f>
         <v>185.91603519099732</v>
       </c>
-      <c r="M30" s="25">
+      <c r="M30" s="24">
         <f>L30/D30</f>
         <v>0.88668920654146366</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B31" s="24">
+      <c r="B31" s="23">
         <f>SUM(B28:B30)</f>
         <v>447.55806616980158</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C31" s="19">
         <f>SUM(C28:C30)</f>
         <v>500</v>
       </c>
-      <c r="D31" s="20">
+      <c r="D31" s="19">
         <f>SUM(D28:D30)</f>
         <v>947.55806616980158</v>
       </c>
-      <c r="E31" s="23">
+      <c r="E31" s="22">
         <f>SUM(E28:E30)</f>
         <v>271.1019661636945</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F31" s="21">
         <f>SUM(F28:F30)</f>
         <v>228.8980338363055</v>
       </c>
       <c r="G31" s="10"/>
-      <c r="H31" s="21">
+      <c r="H31" s="20">
         <f>SUM(H28:H30)</f>
         <v>718.66003233349613</v>
       </c>
-      <c r="I31" s="20">
+      <c r="I31" s="19">
         <f>F31/H31</f>
         <v>0.31850669793486547</v>
       </c>
-      <c r="J31" s="20">
+      <c r="J31" s="19">
         <f>SUM(J28:J30)</f>
         <v>228.8980338363055</v>
       </c>
-      <c r="K31" s="20">
+      <c r="K31" s="19">
         <f>SUM(K28:K30)</f>
         <v>0</v>
       </c>
-      <c r="L31" s="20">
+      <c r="L31" s="19">
         <f>SUM(L28:L30)</f>
         <v>947.55806616980158</v>
       </c>
-      <c r="M31" s="19"/>
+      <c r="M31" s="18"/>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H33" t="s">

</xml_diff>

<commit_message>
Fixed bug with Expanded Reproduction
</commit_message>
<xml_diff>
--- a/docs/spreadsheet illustrations.xlsx
+++ b/docs/spreadsheet illustrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afree\eclipse-workspace\capitalism-9.0\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA01C68-E24D-4130-A713-F324D2975AB6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADA3D89-7F1F-4572-8F9A-E2699B17EA35}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25602" windowHeight="10380" firstSheet="1" activeTab="3" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25602" windowHeight="10380" firstSheet="1" activeTab="4" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Reproduction" sheetId="9" r:id="rId1"/>
@@ -2980,8 +2980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C77ED3-DCBF-4325-9E6B-9BF828DE079E}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3148,11 +3148,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93B651D-F4FB-4BF9-BD8B-3835EA09B3FA}">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3162,7 +3162,7 @@
     <col min="10" max="10" width="10.3671875" customWidth="1"/>
     <col min="11" max="13" width="11.3125" customWidth="1"/>
     <col min="14" max="14" width="8.9453125" style="3"/>
-    <col min="18" max="18" width="11.41796875" customWidth="1"/>
+    <col min="18" max="18" width="13.3125" customWidth="1"/>
     <col min="19" max="19" width="10.20703125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>